<commit_message>
Start of 2023-24 combined analyses
</commit_message>
<xml_diff>
--- a/Input/2023_trap_moth_counts9.xlsx
+++ b/Input/2023_trap_moth_counts9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Noa/Documents/Documents - MacBook Air/PhD/R:Stats:GIS/RStudio/R_Workspace/Pheromone_trap_code/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9342412-C8FE-D348-BCC3-E66E65D9E4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B86BFD-B488-B247-81A2-BCE6EF603709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28400" windowHeight="15800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="520" windowWidth="25220" windowHeight="13940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11847,8 +11847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAAD88A-4CAD-744A-A492-1B588C3F1501}">
   <dimension ref="A1:AA1045"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q103"/>
     </sheetView>
   </sheetViews>
@@ -12058,7 +12058,7 @@
       </c>
       <c r="O3" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>76.563895328822809</v>
+        <v>71.364261329822511</v>
       </c>
       <c r="P3" s="29" t="s">
         <v>249</v>
@@ -12072,7 +12072,7 @@
       </c>
       <c r="S3" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>115.81389532882281</v>
+        <v>110.61426132982251</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>178</v>
@@ -12188,7 +12188,7 @@
       </c>
       <c r="O5" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>73.727230756900539</v>
+        <v>55.816713341567706</v>
       </c>
       <c r="P5" s="29" t="s">
         <v>248</v>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="S5" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>127.22723075690054</v>
+        <v>109.31671334156771</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>176</v>
@@ -12251,7 +12251,7 @@
       </c>
       <c r="O6" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>96.205707715433476</v>
+        <v>93.953865003545786</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>248</v>
@@ -12265,7 +12265,7 @@
       </c>
       <c r="S6" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>96.205707715433476</v>
+        <v>93.953865003545786</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>53</v>
@@ -12322,7 +12322,7 @@
       </c>
       <c r="O7" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>55.049434719826358</v>
+        <v>61.550659280924258</v>
       </c>
       <c r="P7" s="29" t="s">
         <v>249</v>
@@ -12336,7 +12336,7 @@
       </c>
       <c r="S7" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>93.049434719826365</v>
+        <v>99.550659280924265</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>180</v>
@@ -12874,7 +12874,7 @@
       </c>
       <c r="O16" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>5.0403715204524691</v>
+        <v>0.59970605571361069</v>
       </c>
       <c r="P16" s="26" t="s">
         <v>250</v>
@@ -12888,7 +12888,7 @@
       </c>
       <c r="S16" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>51.290371520452467</v>
+        <v>46.849706055713611</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>195</v>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="O17" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>13.578953768382068</v>
+        <v>6.6763150193340364</v>
       </c>
       <c r="P17" s="26" t="s">
         <v>249</v>
@@ -12956,7 +12956,7 @@
       </c>
       <c r="S17" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>64.578953768382064</v>
+        <v>57.676315019334034</v>
       </c>
       <c r="T17" s="5" t="s">
         <v>201</v>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="O18" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>56.766320634742094</v>
+        <v>66.541198150482117</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>249</v>
@@ -13012,7 +13012,7 @@
       </c>
       <c r="S18" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>56.766320634742094</v>
+        <v>66.541198150482117</v>
       </c>
       <c r="V18" s="5" t="s">
         <v>199</v>
@@ -13122,7 +13122,7 @@
       </c>
       <c r="O20" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>5.1350106040315042</v>
+        <v>4.9640703612643957</v>
       </c>
       <c r="P20" s="26" t="s">
         <v>250</v>
@@ -13136,7 +13136,7 @@
       </c>
       <c r="S20" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>30.385010604031503</v>
+        <v>30.214070361264397</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>43</v>
@@ -13193,7 +13193,7 @@
       </c>
       <c r="O21" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>14.872553144665053</v>
+        <v>7.8082278577437823</v>
       </c>
       <c r="P21" s="26" t="s">
         <v>252</v>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="S21" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>30.372553144665055</v>
+        <v>23.30822785774378</v>
       </c>
       <c r="V21" s="5" t="s">
         <v>13</v>
@@ -13379,7 +13379,7 @@
       </c>
       <c r="O24" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>1.4799722732476637</v>
+        <v>15.372771917969391</v>
       </c>
       <c r="P24" s="26" t="s">
         <v>250</v>
@@ -13393,7 +13393,7 @@
       </c>
       <c r="S24" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>41.979972273247661</v>
+        <v>55.872771917969388</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -13559,7 +13559,7 @@
       </c>
       <c r="O27" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>48.437870029877452</v>
+        <v>27.245857705720532</v>
       </c>
       <c r="P27" s="29" t="s">
         <v>250</v>
@@ -13573,7 +13573,7 @@
       </c>
       <c r="S27" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>66.937870029877445</v>
+        <v>45.745857705720532</v>
       </c>
       <c r="T27" s="5" t="s">
         <v>164</v>
@@ -13630,7 +13630,7 @@
       </c>
       <c r="O28" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>76.510125982788367</v>
+        <v>75.958615493831843</v>
       </c>
       <c r="P28" s="29" t="s">
         <v>249</v>
@@ -13644,7 +13644,7 @@
       </c>
       <c r="S28" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>112.51012598278837</v>
+        <v>111.95861549383184</v>
       </c>
       <c r="T28" s="5" t="s">
         <v>154</v>
@@ -13763,7 +13763,7 @@
       </c>
       <c r="O30" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>113.85208875693183</v>
+        <v>113.98966423123703</v>
       </c>
       <c r="P30" s="29" t="s">
         <v>249</v>
@@ -13777,7 +13777,7 @@
       </c>
       <c r="S30" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>120.85208875693183</v>
+        <v>120.98966423123703</v>
       </c>
       <c r="T30" s="26" t="s">
         <v>240</v>
@@ -14235,7 +14235,7 @@
       </c>
       <c r="O38" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>12.946620336429579</v>
+        <v>7.1991936410682476</v>
       </c>
       <c r="P38" s="28" t="s">
         <v>250</v>
@@ -14249,7 +14249,7 @@
       </c>
       <c r="S38" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>40.446620336429575</v>
+        <v>34.699193641068248</v>
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
@@ -14363,7 +14363,7 @@
       </c>
       <c r="O40" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>99.62599354096767</v>
+        <v>102.69212244673488</v>
       </c>
       <c r="P40" s="29" t="s">
         <v>248</v>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="S40" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>99.62599354096767</v>
+        <v>102.69212244673488</v>
       </c>
       <c r="V40" s="5" t="s">
         <v>99</v>
@@ -14426,7 +14426,7 @@
       </c>
       <c r="O41" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>117.79333442837455</v>
+        <v>94.600951924900201</v>
       </c>
       <c r="P41" s="29" t="s">
         <v>248</v>
@@ -14440,7 +14440,7 @@
       </c>
       <c r="S41" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>117.79333442837455</v>
+        <v>94.600951924900201</v>
       </c>
       <c r="V41" s="5" t="s">
         <v>99</v>
@@ -14668,7 +14668,7 @@
       </c>
       <c r="O45" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>7.9646568331014906</v>
+        <v>13.009655167413806</v>
       </c>
       <c r="P45" s="26" t="s">
         <v>252</v>
@@ -14682,7 +14682,7 @@
       </c>
       <c r="S45" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>14.46465683310149</v>
+        <v>19.509655167413804</v>
       </c>
       <c r="V45" s="5" t="s">
         <v>74</v>
@@ -14795,7 +14795,7 @@
       </c>
       <c r="O47" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>66.727589733477842</v>
+        <v>64.984767412740794</v>
       </c>
       <c r="P47" s="29" t="s">
         <v>249</v>
@@ -14809,7 +14809,7 @@
       </c>
       <c r="S47" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>97.727589733477842</v>
+        <v>95.984767412740794</v>
       </c>
       <c r="U47" s="5" t="s">
         <v>70</v>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="O49" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>29.219238977182478</v>
+        <v>48.415963947588352</v>
       </c>
       <c r="P49" s="29" t="s">
         <v>250</v>
@@ -14939,7 +14939,7 @@
       </c>
       <c r="S49" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>29.219238977182478</v>
+        <v>48.415963947588352</v>
       </c>
       <c r="V49" s="5" t="s">
         <v>77</v>
@@ -15100,7 +15100,7 @@
       </c>
       <c r="O52" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>97.550261830919837</v>
+        <v>117.65211241678313</v>
       </c>
       <c r="P52" s="29" t="s">
         <v>248</v>
@@ -15114,7 +15114,7 @@
       </c>
       <c r="S52" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>97.550261830919837</v>
+        <v>117.65211241678313</v>
       </c>
       <c r="V52" s="5" t="s">
         <v>80</v>
@@ -15163,7 +15163,7 @@
       </c>
       <c r="O53" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>105.88592884085739</v>
+        <v>117.60767367864375</v>
       </c>
       <c r="P53" s="29" t="s">
         <v>248</v>
@@ -15177,7 +15177,7 @@
       </c>
       <c r="S53" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>105.88592884085739</v>
+        <v>117.60767367864375</v>
       </c>
       <c r="V53" s="5" t="s">
         <v>84</v>
@@ -15344,7 +15344,7 @@
       </c>
       <c r="O56" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>55.207899788947607</v>
+        <v>51.626144380402621</v>
       </c>
       <c r="P56" t="s">
         <v>249</v>
@@ -15358,7 +15358,7 @@
       </c>
       <c r="S56" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>55.207899788947607</v>
+        <v>51.626144380402621</v>
       </c>
       <c r="V56" s="5" t="s">
         <v>209</v>
@@ -15407,7 +15407,7 @@
       </c>
       <c r="O57" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>89.661831663201312</v>
+        <v>87.142618716580614</v>
       </c>
       <c r="P57" s="29" t="s">
         <v>248</v>
@@ -15421,7 +15421,7 @@
       </c>
       <c r="S57" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>89.661831663201312</v>
+        <v>87.142618716580614</v>
       </c>
       <c r="V57" s="5" t="s">
         <v>214</v>
@@ -15529,7 +15529,7 @@
       </c>
       <c r="O59" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>86.625626581298874</v>
+        <v>112.53474429061771</v>
       </c>
       <c r="P59" s="29" t="s">
         <v>248</v>
@@ -15543,7 +15543,7 @@
       </c>
       <c r="S59" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>86.625626581298874</v>
+        <v>112.53474429061771</v>
       </c>
       <c r="V59" s="5" t="s">
         <v>212</v>
@@ -15707,7 +15707,7 @@
       </c>
       <c r="O62" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>116.61248244396317</v>
+        <v>92.493287742676301</v>
       </c>
       <c r="P62" s="29" t="s">
         <v>248</v>
@@ -15721,7 +15721,7 @@
       </c>
       <c r="S62" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>116.61248244396317</v>
+        <v>92.493287742676301</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>174</v>
@@ -15770,7 +15770,7 @@
       </c>
       <c r="O63" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>118.38147784486782</v>
+        <v>85.42492465429963</v>
       </c>
       <c r="P63" s="29" t="s">
         <v>248</v>
@@ -15784,7 +15784,7 @@
       </c>
       <c r="S63" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>118.38147784486782</v>
+        <v>85.42492465429963</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>174</v>
@@ -15880,7 +15880,7 @@
       </c>
       <c r="O65" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>95.702791974894069</v>
+        <v>98.038747312251175</v>
       </c>
       <c r="P65" s="29" t="s">
         <v>248</v>
@@ -15894,7 +15894,7 @@
       </c>
       <c r="S65" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>95.702791974894069</v>
+        <v>98.038747312251175</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>189</v>
@@ -15943,7 +15943,7 @@
       </c>
       <c r="O66" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>112.09420526943222</v>
+        <v>114.00149182300513</v>
       </c>
       <c r="P66" s="29" t="s">
         <v>248</v>
@@ -15957,7 +15957,7 @@
       </c>
       <c r="S66" s="36">
         <f t="shared" ref="S66:S97" ca="1" si="11">J66+O66</f>
-        <v>112.09420526943222</v>
+        <v>114.00149182300513</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>174</v>
@@ -16121,7 +16121,7 @@
       </c>
       <c r="O69" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>97.778514994260547</v>
+        <v>95.9116155087697</v>
       </c>
       <c r="P69" s="29" t="s">
         <v>248</v>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="S69" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>97.778514994260547</v>
+        <v>95.9116155087697</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>229</v>
@@ -16251,7 +16251,7 @@
       </c>
       <c r="O71" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>21.943268483583527</v>
+        <v>30.171274934441261</v>
       </c>
       <c r="P71" s="29" t="s">
         <v>250</v>
@@ -16265,7 +16265,7 @@
       </c>
       <c r="S71" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>30.943268483583527</v>
+        <v>39.171274934441257</v>
       </c>
       <c r="V71" s="5" t="s">
         <v>226</v>
@@ -16322,7 +16322,7 @@
       </c>
       <c r="O72" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>60.40220954513989</v>
+        <v>53.803093498130551</v>
       </c>
       <c r="P72" s="29" t="s">
         <v>249</v>
@@ -16336,7 +16336,7 @@
       </c>
       <c r="S72" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>89.902209545139897</v>
+        <v>83.303093498130551</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>223</v>
@@ -16388,7 +16388,7 @@
       </c>
       <c r="O73" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>95.629406469929918</v>
+        <v>109.82301737230566</v>
       </c>
       <c r="P73" s="29" t="s">
         <v>248</v>
@@ -16402,7 +16402,7 @@
       </c>
       <c r="S73" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>95.629406469929918</v>
+        <v>109.82301737230566</v>
       </c>
       <c r="V73" s="5" t="s">
         <v>229</v>
@@ -16699,7 +16699,7 @@
       </c>
       <c r="O78" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>2.012115413608849</v>
+        <v>14.785945142817759</v>
       </c>
       <c r="P78" s="39" t="s">
         <v>248</v>
@@ -16713,7 +16713,7 @@
       </c>
       <c r="S78" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>82.762115413608853</v>
+        <v>95.535945142817752</v>
       </c>
       <c r="V78" s="5" t="s">
         <v>113</v>
@@ -16770,7 +16770,7 @@
       </c>
       <c r="O79" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>5.7649545396017965</v>
+        <v>13.488091514699075</v>
       </c>
       <c r="P79" s="26" t="s">
         <v>249</v>
@@ -16784,7 +16784,7 @@
       </c>
       <c r="S79" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>63.514954539601796</v>
+        <v>71.238091514699079</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>120</v>
@@ -16901,7 +16901,7 @@
       </c>
       <c r="O81" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>31.112000659013766</v>
+        <v>37.678422380738752</v>
       </c>
       <c r="P81" s="29" t="s">
         <v>248</v>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="S81" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>90.362000659013773</v>
+        <v>96.928422380738752</v>
       </c>
       <c r="V81" s="5" t="s">
         <v>18</v>
@@ -17266,7 +17266,7 @@
       </c>
       <c r="O87" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>56.438933879793623</v>
+        <v>73.949307275659095</v>
       </c>
       <c r="P87" s="29" t="s">
         <v>249</v>
@@ -17280,7 +17280,7 @@
       </c>
       <c r="S87" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>90.688933879793623</v>
+        <v>108.19930727565909</v>
       </c>
       <c r="T87" s="5">
         <v>0</v>
@@ -17400,7 +17400,7 @@
       </c>
       <c r="O89" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>17.776199987451381</v>
+        <v>0.75339160664497584</v>
       </c>
       <c r="P89" s="27" t="s">
         <v>249</v>
@@ -17414,7 +17414,7 @@
       </c>
       <c r="S89" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>68.526199987451378</v>
+        <v>51.503391606644975</v>
       </c>
       <c r="T89" s="26" t="s">
         <v>235</v>
@@ -17537,7 +17537,7 @@
       </c>
       <c r="O91" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>2.5615434275227735</v>
+        <v>18.809226563125204</v>
       </c>
       <c r="P91" s="26" t="s">
         <v>250</v>
@@ -17551,7 +17551,7 @@
       </c>
       <c r="S91" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>34.811543427522771</v>
+        <v>51.059226563125208</v>
       </c>
       <c r="T91" s="5" t="s">
         <v>37</v>
@@ -17842,7 +17842,7 @@
       </c>
       <c r="O96" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>82.969921898699937</v>
+        <v>97.650543273074376</v>
       </c>
       <c r="P96" s="29" t="s">
         <v>248</v>
@@ -17856,7 +17856,7 @@
       </c>
       <c r="S96" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>82.969921898699937</v>
+        <v>97.650543273074376</v>
       </c>
       <c r="V96" s="5" t="s">
         <v>145</v>
@@ -17913,7 +17913,7 @@
       </c>
       <c r="O97" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>116.36007006306757</v>
+        <v>110.97018206106195</v>
       </c>
       <c r="P97" s="29" t="s">
         <v>248</v>
@@ -17927,7 +17927,7 @@
       </c>
       <c r="S97" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>157.36007006306755</v>
+        <v>151.97018206106196</v>
       </c>
       <c r="V97" s="5" t="s">
         <v>145</v>
@@ -18046,7 +18046,7 @@
       </c>
       <c r="O99" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>75.421325860002042</v>
+        <v>73.356170931538657</v>
       </c>
       <c r="P99" s="29" t="s">
         <v>248</v>
@@ -18060,7 +18060,7 @@
       </c>
       <c r="S99" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>139.67132586000204</v>
+        <v>137.60617093153866</v>
       </c>
       <c r="T99" s="5" t="s">
         <v>133</v>
@@ -18176,7 +18176,7 @@
       </c>
       <c r="O101" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>23.802134037236325</v>
+        <v>32.869764623316811</v>
       </c>
       <c r="P101" s="29" t="s">
         <v>250</v>
@@ -18190,7 +18190,7 @@
       </c>
       <c r="S101" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>31.802134037236325</v>
+        <v>40.869764623316811</v>
       </c>
       <c r="T101" s="26" t="s">
         <v>239</v>
@@ -18315,7 +18315,7 @@
       </c>
       <c r="O103" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>14.951741546731848</v>
+        <v>18.570878519964776</v>
       </c>
       <c r="P103" s="26" t="s">
         <v>250</v>
@@ -18329,7 +18329,7 @@
       </c>
       <c r="S103" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>55.201741546731846</v>
+        <v>58.820878519964779</v>
       </c>
       <c r="T103" s="5" t="s">
         <v>137</v>
@@ -21699,10 +21699,10 @@
   <dimension ref="A1:V119"/>
   <sheetViews>
     <sheetView zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="11" ySplit="16" topLeftCell="P17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="16" topLeftCell="T92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8:D13"/>
+      <selection pane="bottomRight" activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -21719,7 +21719,7 @@
     <col min="11" max="13" width="10.83203125" style="61"/>
     <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="49" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="41.1640625" style="40" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="40" customWidth="1"/>
     <col min="17" max="17" width="18.6640625" customWidth="1"/>
     <col min="18" max="18" width="39.5" style="49" customWidth="1"/>
     <col min="19" max="19" width="17" style="73" bestFit="1" customWidth="1"/>
@@ -28265,8 +28265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA127177-25C6-664D-9F19-42DDA7C8C436}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Create new graphs and output for this data
</commit_message>
<xml_diff>
--- a/Input/2023_trap_moth_counts9.xlsx
+++ b/Input/2023_trap_moth_counts9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Noa/Documents/Documents - MacBook Air/PhD/R:Stats:GIS/RStudio/R_Workspace/Pheromone_trap_code/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B86BFD-B488-B247-81A2-BCE6EF603709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0321951-0B69-3C41-9355-50448F9AD34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="520" windowWidth="25220" windowHeight="13940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3440" yWindow="520" windowWidth="25220" windowHeight="13940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12058,7 +12058,7 @@
       </c>
       <c r="O3" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>71.364261329822511</v>
+        <v>54.684171499922918</v>
       </c>
       <c r="P3" s="29" t="s">
         <v>249</v>
@@ -12072,7 +12072,7 @@
       </c>
       <c r="S3" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>110.61426132982251</v>
+        <v>93.934171499922911</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>178</v>
@@ -12188,7 +12188,7 @@
       </c>
       <c r="O5" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>55.816713341567706</v>
+        <v>57.851664714964578</v>
       </c>
       <c r="P5" s="29" t="s">
         <v>248</v>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="S5" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>109.31671334156771</v>
+        <v>111.35166471496458</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>176</v>
@@ -12251,7 +12251,7 @@
       </c>
       <c r="O6" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>93.953865003545786</v>
+        <v>106.61349679379519</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>248</v>
@@ -12265,7 +12265,7 @@
       </c>
       <c r="S6" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>93.953865003545786</v>
+        <v>106.61349679379519</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>53</v>
@@ -12322,7 +12322,7 @@
       </c>
       <c r="O7" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>61.550659280924258</v>
+        <v>61.78633687094888</v>
       </c>
       <c r="P7" s="29" t="s">
         <v>249</v>
@@ -12336,7 +12336,7 @@
       </c>
       <c r="S7" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>99.550659280924265</v>
+        <v>99.786336870948873</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>180</v>
@@ -12874,7 +12874,7 @@
       </c>
       <c r="O16" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>0.59970605571361069</v>
+        <v>6.1830460813584383</v>
       </c>
       <c r="P16" s="26" t="s">
         <v>250</v>
@@ -12888,7 +12888,7 @@
       </c>
       <c r="S16" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>46.849706055713611</v>
+        <v>52.433046081358441</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>195</v>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="O17" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>6.6763150193340364</v>
+        <v>1.5327729288352536</v>
       </c>
       <c r="P17" s="26" t="s">
         <v>249</v>
@@ -12956,7 +12956,7 @@
       </c>
       <c r="S17" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>57.676315019334034</v>
+        <v>52.532772928835257</v>
       </c>
       <c r="T17" s="5" t="s">
         <v>201</v>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="O18" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>66.541198150482117</v>
+        <v>54.681583437263498</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>249</v>
@@ -13012,7 +13012,7 @@
       </c>
       <c r="S18" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>66.541198150482117</v>
+        <v>54.681583437263498</v>
       </c>
       <c r="V18" s="5" t="s">
         <v>199</v>
@@ -13122,7 +13122,7 @@
       </c>
       <c r="O20" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>4.9640703612643957</v>
+        <v>1.2987676852678556</v>
       </c>
       <c r="P20" s="26" t="s">
         <v>250</v>
@@ -13136,7 +13136,7 @@
       </c>
       <c r="S20" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>30.214070361264397</v>
+        <v>26.548767685267855</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>43</v>
@@ -13193,7 +13193,7 @@
       </c>
       <c r="O21" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>7.8082278577437823</v>
+        <v>11.044197403468985</v>
       </c>
       <c r="P21" s="26" t="s">
         <v>252</v>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="S21" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>23.30822785774378</v>
+        <v>26.544197403468985</v>
       </c>
       <c r="V21" s="5" t="s">
         <v>13</v>
@@ -13379,7 +13379,7 @@
       </c>
       <c r="O24" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>15.372771917969391</v>
+        <v>1.1857098871866794</v>
       </c>
       <c r="P24" s="26" t="s">
         <v>250</v>
@@ -13393,7 +13393,7 @@
       </c>
       <c r="S24" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>55.872771917969388</v>
+        <v>41.685709887186682</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -13559,7 +13559,7 @@
       </c>
       <c r="O27" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>27.245857705720532</v>
+        <v>38.818202795081291</v>
       </c>
       <c r="P27" s="29" t="s">
         <v>250</v>
@@ -13573,7 +13573,7 @@
       </c>
       <c r="S27" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>45.745857705720532</v>
+        <v>57.318202795081291</v>
       </c>
       <c r="T27" s="5" t="s">
         <v>164</v>
@@ -13630,7 +13630,7 @@
       </c>
       <c r="O28" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>75.958615493831843</v>
+        <v>73.433079321393066</v>
       </c>
       <c r="P28" s="29" t="s">
         <v>249</v>
@@ -13644,7 +13644,7 @@
       </c>
       <c r="S28" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>111.95861549383184</v>
+        <v>109.43307932139307</v>
       </c>
       <c r="T28" s="5" t="s">
         <v>154</v>
@@ -13763,7 +13763,7 @@
       </c>
       <c r="O30" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>113.98966423123703</v>
+        <v>82.439654343896123</v>
       </c>
       <c r="P30" s="29" t="s">
         <v>249</v>
@@ -13777,7 +13777,7 @@
       </c>
       <c r="S30" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>120.98966423123703</v>
+        <v>89.439654343896123</v>
       </c>
       <c r="T30" s="26" t="s">
         <v>240</v>
@@ -14235,7 +14235,7 @@
       </c>
       <c r="O38" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>7.1991936410682476</v>
+        <v>6.0429102565901491</v>
       </c>
       <c r="P38" s="28" t="s">
         <v>250</v>
@@ -14249,7 +14249,7 @@
       </c>
       <c r="S38" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>34.699193641068248</v>
+        <v>33.542910256590147</v>
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
@@ -14363,7 +14363,7 @@
       </c>
       <c r="O40" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>102.69212244673488</v>
+        <v>97.692282461685565</v>
       </c>
       <c r="P40" s="29" t="s">
         <v>248</v>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="S40" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>102.69212244673488</v>
+        <v>97.692282461685565</v>
       </c>
       <c r="V40" s="5" t="s">
         <v>99</v>
@@ -14426,7 +14426,7 @@
       </c>
       <c r="O41" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>94.600951924900201</v>
+        <v>101.13016619002636</v>
       </c>
       <c r="P41" s="29" t="s">
         <v>248</v>
@@ -14440,7 +14440,7 @@
       </c>
       <c r="S41" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>94.600951924900201</v>
+        <v>101.13016619002636</v>
       </c>
       <c r="V41" s="5" t="s">
         <v>99</v>
@@ -14668,7 +14668,7 @@
       </c>
       <c r="O45" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>13.009655167413806</v>
+        <v>17.213036080804223</v>
       </c>
       <c r="P45" s="26" t="s">
         <v>252</v>
@@ -14682,7 +14682,7 @@
       </c>
       <c r="S45" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>19.509655167413804</v>
+        <v>23.713036080804223</v>
       </c>
       <c r="V45" s="5" t="s">
         <v>74</v>
@@ -14795,7 +14795,7 @@
       </c>
       <c r="O47" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>64.984767412740794</v>
+        <v>65.413198093095986</v>
       </c>
       <c r="P47" s="29" t="s">
         <v>249</v>
@@ -14809,7 +14809,7 @@
       </c>
       <c r="S47" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>95.984767412740794</v>
+        <v>96.413198093095986</v>
       </c>
       <c r="U47" s="5" t="s">
         <v>70</v>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="O49" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>48.415963947588352</v>
+        <v>20.610517237301817</v>
       </c>
       <c r="P49" s="29" t="s">
         <v>250</v>
@@ -14939,7 +14939,7 @@
       </c>
       <c r="S49" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>48.415963947588352</v>
+        <v>20.610517237301817</v>
       </c>
       <c r="V49" s="5" t="s">
         <v>77</v>
@@ -15100,7 +15100,7 @@
       </c>
       <c r="O52" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>117.65211241678313</v>
+        <v>109.29056649587649</v>
       </c>
       <c r="P52" s="29" t="s">
         <v>248</v>
@@ -15114,7 +15114,7 @@
       </c>
       <c r="S52" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>117.65211241678313</v>
+        <v>109.29056649587649</v>
       </c>
       <c r="V52" s="5" t="s">
         <v>80</v>
@@ -15163,7 +15163,7 @@
       </c>
       <c r="O53" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>117.60767367864375</v>
+        <v>81.457998990348571</v>
       </c>
       <c r="P53" s="29" t="s">
         <v>248</v>
@@ -15177,7 +15177,7 @@
       </c>
       <c r="S53" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>117.60767367864375</v>
+        <v>81.457998990348571</v>
       </c>
       <c r="V53" s="5" t="s">
         <v>84</v>
@@ -15344,7 +15344,7 @@
       </c>
       <c r="O56" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>51.626144380402621</v>
+        <v>53.52757504879429</v>
       </c>
       <c r="P56" t="s">
         <v>249</v>
@@ -15358,7 +15358,7 @@
       </c>
       <c r="S56" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>51.626144380402621</v>
+        <v>53.52757504879429</v>
       </c>
       <c r="V56" s="5" t="s">
         <v>209</v>
@@ -15407,7 +15407,7 @@
       </c>
       <c r="O57" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>87.142618716580614</v>
+        <v>95.380750395823014</v>
       </c>
       <c r="P57" s="29" t="s">
         <v>248</v>
@@ -15421,7 +15421,7 @@
       </c>
       <c r="S57" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>87.142618716580614</v>
+        <v>95.380750395823014</v>
       </c>
       <c r="V57" s="5" t="s">
         <v>214</v>
@@ -15529,7 +15529,7 @@
       </c>
       <c r="O59" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>112.53474429061771</v>
+        <v>80.431818423522756</v>
       </c>
       <c r="P59" s="29" t="s">
         <v>248</v>
@@ -15543,7 +15543,7 @@
       </c>
       <c r="S59" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>112.53474429061771</v>
+        <v>80.431818423522756</v>
       </c>
       <c r="V59" s="5" t="s">
         <v>212</v>
@@ -15707,7 +15707,7 @@
       </c>
       <c r="O62" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>92.493287742676301</v>
+        <v>108.19805339884896</v>
       </c>
       <c r="P62" s="29" t="s">
         <v>248</v>
@@ -15721,7 +15721,7 @@
       </c>
       <c r="S62" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>92.493287742676301</v>
+        <v>108.19805339884896</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>174</v>
@@ -15770,7 +15770,7 @@
       </c>
       <c r="O63" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>85.42492465429963</v>
+        <v>115.97226825282458</v>
       </c>
       <c r="P63" s="29" t="s">
         <v>248</v>
@@ -15784,7 +15784,7 @@
       </c>
       <c r="S63" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>85.42492465429963</v>
+        <v>115.97226825282458</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>174</v>
@@ -15880,7 +15880,7 @@
       </c>
       <c r="O65" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>98.038747312251175</v>
+        <v>96.532675305609786</v>
       </c>
       <c r="P65" s="29" t="s">
         <v>248</v>
@@ -15894,7 +15894,7 @@
       </c>
       <c r="S65" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>98.038747312251175</v>
+        <v>96.532675305609786</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>189</v>
@@ -15943,7 +15943,7 @@
       </c>
       <c r="O66" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>114.00149182300513</v>
+        <v>100.20816028684374</v>
       </c>
       <c r="P66" s="29" t="s">
         <v>248</v>
@@ -15957,7 +15957,7 @@
       </c>
       <c r="S66" s="36">
         <f t="shared" ref="S66:S97" ca="1" si="11">J66+O66</f>
-        <v>114.00149182300513</v>
+        <v>100.20816028684374</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>174</v>
@@ -16121,7 +16121,7 @@
       </c>
       <c r="O69" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>95.9116155087697</v>
+        <v>91.594599901336892</v>
       </c>
       <c r="P69" s="29" t="s">
         <v>248</v>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="S69" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>95.9116155087697</v>
+        <v>91.594599901336892</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>229</v>
@@ -16251,7 +16251,7 @@
       </c>
       <c r="O71" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>30.171274934441261</v>
+        <v>43.540244951945105</v>
       </c>
       <c r="P71" s="29" t="s">
         <v>250</v>
@@ -16265,7 +16265,7 @@
       </c>
       <c r="S71" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>39.171274934441257</v>
+        <v>52.540244951945105</v>
       </c>
       <c r="V71" s="5" t="s">
         <v>226</v>
@@ -16322,7 +16322,7 @@
       </c>
       <c r="O72" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>53.803093498130551</v>
+        <v>70.437571169700306</v>
       </c>
       <c r="P72" s="29" t="s">
         <v>249</v>
@@ -16336,7 +16336,7 @@
       </c>
       <c r="S72" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>83.303093498130551</v>
+        <v>99.937571169700306</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>223</v>
@@ -16388,7 +16388,7 @@
       </c>
       <c r="O73" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>109.82301737230566</v>
+        <v>104.90086204632834</v>
       </c>
       <c r="P73" s="29" t="s">
         <v>248</v>
@@ -16402,7 +16402,7 @@
       </c>
       <c r="S73" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>109.82301737230566</v>
+        <v>104.90086204632834</v>
       </c>
       <c r="V73" s="5" t="s">
         <v>229</v>
@@ -16699,7 +16699,7 @@
       </c>
       <c r="O78" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>14.785945142817759</v>
+        <v>1.8251487766230476</v>
       </c>
       <c r="P78" s="39" t="s">
         <v>248</v>
@@ -16713,7 +16713,7 @@
       </c>
       <c r="S78" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>95.535945142817752</v>
+        <v>82.575148776623053</v>
       </c>
       <c r="V78" s="5" t="s">
         <v>113</v>
@@ -16770,7 +16770,7 @@
       </c>
       <c r="O79" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>13.488091514699075</v>
+        <v>3.0252200635762461</v>
       </c>
       <c r="P79" s="26" t="s">
         <v>249</v>
@@ -16784,7 +16784,7 @@
       </c>
       <c r="S79" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>71.238091514699079</v>
+        <v>60.775220063576249</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>120</v>
@@ -16901,7 +16901,7 @@
       </c>
       <c r="O81" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>37.678422380738752</v>
+        <v>26.645511941442759</v>
       </c>
       <c r="P81" s="29" t="s">
         <v>248</v>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="S81" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>96.928422380738752</v>
+        <v>85.895511941442763</v>
       </c>
       <c r="V81" s="5" t="s">
         <v>18</v>
@@ -17266,7 +17266,7 @@
       </c>
       <c r="O87" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>73.949307275659095</v>
+        <v>70.967812503065915</v>
       </c>
       <c r="P87" s="29" t="s">
         <v>249</v>
@@ -17280,7 +17280,7 @@
       </c>
       <c r="S87" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>108.19930727565909</v>
+        <v>105.21781250306591</v>
       </c>
       <c r="T87" s="5">
         <v>0</v>
@@ -17400,7 +17400,7 @@
       </c>
       <c r="O89" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>0.75339160664497584</v>
+        <v>10.001217556579114</v>
       </c>
       <c r="P89" s="27" t="s">
         <v>249</v>
@@ -17414,7 +17414,7 @@
       </c>
       <c r="S89" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>51.503391606644975</v>
+        <v>60.751217556579114</v>
       </c>
       <c r="T89" s="26" t="s">
         <v>235</v>
@@ -17537,7 +17537,7 @@
       </c>
       <c r="O91" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>18.809226563125204</v>
+        <v>16.648485893013749</v>
       </c>
       <c r="P91" s="26" t="s">
         <v>250</v>
@@ -17551,7 +17551,7 @@
       </c>
       <c r="S91" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>51.059226563125208</v>
+        <v>48.898485893013749</v>
       </c>
       <c r="T91" s="5" t="s">
         <v>37</v>
@@ -17842,7 +17842,7 @@
       </c>
       <c r="O96" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>97.650543273074376</v>
+        <v>82.924642966298478</v>
       </c>
       <c r="P96" s="29" t="s">
         <v>248</v>
@@ -17856,7 +17856,7 @@
       </c>
       <c r="S96" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>97.650543273074376</v>
+        <v>82.924642966298478</v>
       </c>
       <c r="V96" s="5" t="s">
         <v>145</v>
@@ -17913,7 +17913,7 @@
       </c>
       <c r="O97" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>110.97018206106195</v>
+        <v>89.513861799055036</v>
       </c>
       <c r="P97" s="29" t="s">
         <v>248</v>
@@ -17927,7 +17927,7 @@
       </c>
       <c r="S97" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>151.97018206106196</v>
+        <v>130.51386179905504</v>
       </c>
       <c r="V97" s="5" t="s">
         <v>145</v>
@@ -18046,7 +18046,7 @@
       </c>
       <c r="O99" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>73.356170931538657</v>
+        <v>61.130196959359424</v>
       </c>
       <c r="P99" s="29" t="s">
         <v>248</v>
@@ -18060,7 +18060,7 @@
       </c>
       <c r="S99" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>137.60617093153866</v>
+        <v>125.38019695935942</v>
       </c>
       <c r="T99" s="5" t="s">
         <v>133</v>
@@ -18176,7 +18176,7 @@
       </c>
       <c r="O101" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>32.869764623316811</v>
+        <v>43.694337130762392</v>
       </c>
       <c r="P101" s="29" t="s">
         <v>250</v>
@@ -18190,7 +18190,7 @@
       </c>
       <c r="S101" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>40.869764623316811</v>
+        <v>51.694337130762392</v>
       </c>
       <c r="T101" s="26" t="s">
         <v>239</v>
@@ -18315,7 +18315,7 @@
       </c>
       <c r="O103" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>18.570878519964776</v>
+        <v>8.3357952728733071</v>
       </c>
       <c r="P103" s="26" t="s">
         <v>250</v>
@@ -18329,7 +18329,7 @@
       </c>
       <c r="S103" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>58.820878519964779</v>
+        <v>48.585795272873305</v>
       </c>
       <c r="T103" s="5" t="s">
         <v>137</v>
@@ -21699,10 +21699,10 @@
   <dimension ref="A1:V119"/>
   <sheetViews>
     <sheetView zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="11" ySplit="16" topLeftCell="T92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="16" topLeftCell="U101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="I97" sqref="I97"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28265,8 +28265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA127177-25C6-664D-9F19-42DDA7C8C436}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
processing Censored Data w Bayesian stats
</commit_message>
<xml_diff>
--- a/Input/2023_trap_moth_counts9.xlsx
+++ b/Input/2023_trap_moth_counts9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Noa/Documents/Documents - MacBook Air/PhD/R:Stats:GIS/RStudio/R_Workspace/Pheromone_trap_code/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0321951-0B69-3C41-9355-50448F9AD34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD639C1E-B9AF-4844-AE40-B5C047184387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3440" yWindow="520" windowWidth="25220" windowHeight="13940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12720" yWindow="520" windowWidth="15940" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11847,9 +11847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAAD88A-4CAD-744A-A492-1B588C3F1501}">
   <dimension ref="A1:AA1045"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q103"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12058,7 +12058,7 @@
       </c>
       <c r="O3" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>54.684171499922918</v>
+        <v>66.136577632857652</v>
       </c>
       <c r="P3" s="29" t="s">
         <v>249</v>
@@ -12072,7 +12072,7 @@
       </c>
       <c r="S3" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>93.934171499922911</v>
+        <v>105.38657763285765</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>178</v>
@@ -12188,7 +12188,7 @@
       </c>
       <c r="O5" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>57.851664714964578</v>
+        <v>58.969740446242653</v>
       </c>
       <c r="P5" s="29" t="s">
         <v>248</v>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="S5" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>111.35166471496458</v>
+        <v>112.46974044624265</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>176</v>
@@ -12251,7 +12251,7 @@
       </c>
       <c r="O6" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>106.61349679379519</v>
+        <v>117.63355026477697</v>
       </c>
       <c r="P6" s="29" t="s">
         <v>248</v>
@@ -12265,7 +12265,7 @@
       </c>
       <c r="S6" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>106.61349679379519</v>
+        <v>117.63355026477697</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>53</v>
@@ -12322,7 +12322,7 @@
       </c>
       <c r="O7" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>61.78633687094888</v>
+        <v>76.078271087612706</v>
       </c>
       <c r="P7" s="29" t="s">
         <v>249</v>
@@ -12336,7 +12336,7 @@
       </c>
       <c r="S7" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>99.786336870948873</v>
+        <v>114.07827108761271</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>180</v>
@@ -12874,7 +12874,7 @@
       </c>
       <c r="O16" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>6.1830460813584383</v>
+        <v>1.6601872286192365E-2</v>
       </c>
       <c r="P16" s="26" t="s">
         <v>250</v>
@@ -12888,7 +12888,7 @@
       </c>
       <c r="S16" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>52.433046081358441</v>
+        <v>46.266601872286195</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>195</v>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="O17" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>1.5327729288352536</v>
+        <v>16.354837067557074</v>
       </c>
       <c r="P17" s="26" t="s">
         <v>249</v>
@@ -12956,7 +12956,7 @@
       </c>
       <c r="S17" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>52.532772928835257</v>
+        <v>67.354837067557071</v>
       </c>
       <c r="T17" s="5" t="s">
         <v>201</v>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="O18" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>54.681583437263498</v>
+        <v>66.211994473771171</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>249</v>
@@ -13012,7 +13012,7 @@
       </c>
       <c r="S18" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>54.681583437263498</v>
+        <v>66.211994473771171</v>
       </c>
       <c r="V18" s="5" t="s">
         <v>199</v>
@@ -13122,7 +13122,7 @@
       </c>
       <c r="O20" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>1.2987676852678556</v>
+        <v>16.033411151633743</v>
       </c>
       <c r="P20" s="26" t="s">
         <v>250</v>
@@ -13136,7 +13136,7 @@
       </c>
       <c r="S20" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>26.548767685267855</v>
+        <v>41.283411151633743</v>
       </c>
       <c r="T20" s="5" t="s">
         <v>43</v>
@@ -13193,7 +13193,7 @@
       </c>
       <c r="O21" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>11.044197403468985</v>
+        <v>6.6670806061717522</v>
       </c>
       <c r="P21" s="26" t="s">
         <v>252</v>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="S21" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>26.544197403468985</v>
+        <v>22.167080606171751</v>
       </c>
       <c r="V21" s="5" t="s">
         <v>13</v>
@@ -13379,7 +13379,7 @@
       </c>
       <c r="O24" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>1.1857098871866794</v>
+        <v>10.250139628530317</v>
       </c>
       <c r="P24" s="26" t="s">
         <v>250</v>
@@ -13393,7 +13393,7 @@
       </c>
       <c r="S24" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>41.685709887186682</v>
+        <v>50.75013962853032</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -13559,7 +13559,7 @@
       </c>
       <c r="O27" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>38.818202795081291</v>
+        <v>28.484082317314474</v>
       </c>
       <c r="P27" s="29" t="s">
         <v>250</v>
@@ -13573,7 +13573,7 @@
       </c>
       <c r="S27" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>57.318202795081291</v>
+        <v>46.984082317314474</v>
       </c>
       <c r="T27" s="5" t="s">
         <v>164</v>
@@ -13630,7 +13630,7 @@
       </c>
       <c r="O28" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>73.433079321393066</v>
+        <v>73.541141232648471</v>
       </c>
       <c r="P28" s="29" t="s">
         <v>249</v>
@@ -13644,7 +13644,7 @@
       </c>
       <c r="S28" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>109.43307932139307</v>
+        <v>109.54114123264847</v>
       </c>
       <c r="T28" s="5" t="s">
         <v>154</v>
@@ -13763,7 +13763,7 @@
       </c>
       <c r="O30" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>82.439654343896123</v>
+        <v>106.31926084377756</v>
       </c>
       <c r="P30" s="29" t="s">
         <v>249</v>
@@ -13777,7 +13777,7 @@
       </c>
       <c r="S30" s="36">
         <f t="shared" ca="1" si="2"/>
-        <v>89.439654343896123</v>
+        <v>113.31926084377756</v>
       </c>
       <c r="T30" s="26" t="s">
         <v>240</v>
@@ -14235,7 +14235,7 @@
       </c>
       <c r="O38" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>6.0429102565901491</v>
+        <v>14.884515747584299</v>
       </c>
       <c r="P38" s="28" t="s">
         <v>250</v>
@@ -14249,7 +14249,7 @@
       </c>
       <c r="S38" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>33.542910256590147</v>
+        <v>42.384515747584302</v>
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
@@ -14363,7 +14363,7 @@
       </c>
       <c r="O40" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>97.692282461685565</v>
+        <v>80.274433196011927</v>
       </c>
       <c r="P40" s="29" t="s">
         <v>248</v>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="S40" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>97.692282461685565</v>
+        <v>80.274433196011927</v>
       </c>
       <c r="V40" s="5" t="s">
         <v>99</v>
@@ -14426,7 +14426,7 @@
       </c>
       <c r="O41" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>101.13016619002636</v>
+        <v>98.430007132128239</v>
       </c>
       <c r="P41" s="29" t="s">
         <v>248</v>
@@ -14440,7 +14440,7 @@
       </c>
       <c r="S41" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>101.13016619002636</v>
+        <v>98.430007132128239</v>
       </c>
       <c r="V41" s="5" t="s">
         <v>99</v>
@@ -14668,7 +14668,7 @@
       </c>
       <c r="O45" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>17.213036080804223</v>
+        <v>4.1583936086261986</v>
       </c>
       <c r="P45" s="26" t="s">
         <v>252</v>
@@ -14682,7 +14682,7 @@
       </c>
       <c r="S45" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>23.713036080804223</v>
+        <v>10.658393608626199</v>
       </c>
       <c r="V45" s="5" t="s">
         <v>74</v>
@@ -14795,7 +14795,7 @@
       </c>
       <c r="O47" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>65.413198093095986</v>
+        <v>62.1902217406723</v>
       </c>
       <c r="P47" s="29" t="s">
         <v>249</v>
@@ -14809,7 +14809,7 @@
       </c>
       <c r="S47" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>96.413198093095986</v>
+        <v>93.1902217406723</v>
       </c>
       <c r="U47" s="5" t="s">
         <v>70</v>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="O49" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>20.610517237301817</v>
+        <v>40.878506418582489</v>
       </c>
       <c r="P49" s="29" t="s">
         <v>250</v>
@@ -14939,7 +14939,7 @@
       </c>
       <c r="S49" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>20.610517237301817</v>
+        <v>40.878506418582489</v>
       </c>
       <c r="V49" s="5" t="s">
         <v>77</v>
@@ -15100,7 +15100,7 @@
       </c>
       <c r="O52" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>109.29056649587649</v>
+        <v>89.075062581344781</v>
       </c>
       <c r="P52" s="29" t="s">
         <v>248</v>
@@ -15114,7 +15114,7 @@
       </c>
       <c r="S52" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>109.29056649587649</v>
+        <v>89.075062581344781</v>
       </c>
       <c r="V52" s="5" t="s">
         <v>80</v>
@@ -15163,7 +15163,7 @@
       </c>
       <c r="O53" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>81.457998990348571</v>
+        <v>92.669818224253603</v>
       </c>
       <c r="P53" s="29" t="s">
         <v>248</v>
@@ -15177,7 +15177,7 @@
       </c>
       <c r="S53" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>81.457998990348571</v>
+        <v>92.669818224253603</v>
       </c>
       <c r="V53" s="5" t="s">
         <v>84</v>
@@ -15344,7 +15344,7 @@
       </c>
       <c r="O56" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>53.52757504879429</v>
+        <v>61.410806632312323</v>
       </c>
       <c r="P56" t="s">
         <v>249</v>
@@ -15358,7 +15358,7 @@
       </c>
       <c r="S56" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>53.52757504879429</v>
+        <v>61.410806632312323</v>
       </c>
       <c r="V56" s="5" t="s">
         <v>209</v>
@@ -15407,7 +15407,7 @@
       </c>
       <c r="O57" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>95.380750395823014</v>
+        <v>85.647038526493034</v>
       </c>
       <c r="P57" s="29" t="s">
         <v>248</v>
@@ -15421,7 +15421,7 @@
       </c>
       <c r="S57" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>95.380750395823014</v>
+        <v>85.647038526493034</v>
       </c>
       <c r="V57" s="5" t="s">
         <v>214</v>
@@ -15529,7 +15529,7 @@
       </c>
       <c r="O59" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>80.431818423522756</v>
+        <v>116.46626722499369</v>
       </c>
       <c r="P59" s="29" t="s">
         <v>248</v>
@@ -15543,7 +15543,7 @@
       </c>
       <c r="S59" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>80.431818423522756</v>
+        <v>116.46626722499369</v>
       </c>
       <c r="V59" s="5" t="s">
         <v>212</v>
@@ -15707,7 +15707,7 @@
       </c>
       <c r="O62" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>108.19805339884896</v>
+        <v>94.798595497306479</v>
       </c>
       <c r="P62" s="29" t="s">
         <v>248</v>
@@ -15721,7 +15721,7 @@
       </c>
       <c r="S62" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>108.19805339884896</v>
+        <v>94.798595497306479</v>
       </c>
       <c r="V62" s="5" t="s">
         <v>174</v>
@@ -15770,7 +15770,7 @@
       </c>
       <c r="O63" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>115.97226825282458</v>
+        <v>88.996727983029388</v>
       </c>
       <c r="P63" s="29" t="s">
         <v>248</v>
@@ -15784,7 +15784,7 @@
       </c>
       <c r="S63" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>115.97226825282458</v>
+        <v>88.996727983029388</v>
       </c>
       <c r="V63" s="5" t="s">
         <v>174</v>
@@ -15880,7 +15880,7 @@
       </c>
       <c r="O65" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>96.532675305609786</v>
+        <v>110.34868299952238</v>
       </c>
       <c r="P65" s="29" t="s">
         <v>248</v>
@@ -15894,7 +15894,7 @@
       </c>
       <c r="S65" s="36">
         <f t="shared" ca="1" si="7"/>
-        <v>96.532675305609786</v>
+        <v>110.34868299952238</v>
       </c>
       <c r="V65" s="5" t="s">
         <v>189</v>
@@ -15943,7 +15943,7 @@
       </c>
       <c r="O66" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>100.20816028684374</v>
+        <v>104.29872261302765</v>
       </c>
       <c r="P66" s="29" t="s">
         <v>248</v>
@@ -15957,7 +15957,7 @@
       </c>
       <c r="S66" s="36">
         <f t="shared" ref="S66:S97" ca="1" si="11">J66+O66</f>
-        <v>100.20816028684374</v>
+        <v>104.29872261302765</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>174</v>
@@ -16121,7 +16121,7 @@
       </c>
       <c r="O69" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>91.594599901336892</v>
+        <v>114.0875927799362</v>
       </c>
       <c r="P69" s="29" t="s">
         <v>248</v>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="S69" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>91.594599901336892</v>
+        <v>114.0875927799362</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>229</v>
@@ -16251,7 +16251,7 @@
       </c>
       <c r="O71" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>43.540244951945105</v>
+        <v>25.744513413933607</v>
       </c>
       <c r="P71" s="29" t="s">
         <v>250</v>
@@ -16265,7 +16265,7 @@
       </c>
       <c r="S71" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>52.540244951945105</v>
+        <v>34.744513413933603</v>
       </c>
       <c r="V71" s="5" t="s">
         <v>226</v>
@@ -16322,7 +16322,7 @@
       </c>
       <c r="O72" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>70.437571169700306</v>
+        <v>63.271552246514609</v>
       </c>
       <c r="P72" s="29" t="s">
         <v>249</v>
@@ -16336,7 +16336,7 @@
       </c>
       <c r="S72" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>99.937571169700306</v>
+        <v>92.771552246514602</v>
       </c>
       <c r="V72" s="5" t="s">
         <v>223</v>
@@ -16388,7 +16388,7 @@
       </c>
       <c r="O73" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>104.90086204632834</v>
+        <v>104.46103554218166</v>
       </c>
       <c r="P73" s="29" t="s">
         <v>248</v>
@@ -16402,7 +16402,7 @@
       </c>
       <c r="S73" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>104.90086204632834</v>
+        <v>104.46103554218166</v>
       </c>
       <c r="V73" s="5" t="s">
         <v>229</v>
@@ -16699,7 +16699,7 @@
       </c>
       <c r="O78" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>1.8251487766230476</v>
+        <v>11.618806666139944</v>
       </c>
       <c r="P78" s="39" t="s">
         <v>248</v>
@@ -16713,7 +16713,7 @@
       </c>
       <c r="S78" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>82.575148776623053</v>
+        <v>92.368806666139946</v>
       </c>
       <c r="V78" s="5" t="s">
         <v>113</v>
@@ -16770,7 +16770,7 @@
       </c>
       <c r="O79" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>3.0252200635762461</v>
+        <v>15.89681282214152</v>
       </c>
       <c r="P79" s="26" t="s">
         <v>249</v>
@@ -16784,7 +16784,7 @@
       </c>
       <c r="S79" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>60.775220063576249</v>
+        <v>73.646812822141527</v>
       </c>
       <c r="T79" s="5" t="s">
         <v>120</v>
@@ -16901,7 +16901,7 @@
       </c>
       <c r="O81" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>26.645511941442759</v>
+        <v>38.064663642295912</v>
       </c>
       <c r="P81" s="29" t="s">
         <v>248</v>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="S81" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>85.895511941442763</v>
+        <v>97.314663642295912</v>
       </c>
       <c r="V81" s="5" t="s">
         <v>18</v>
@@ -17266,7 +17266,7 @@
       </c>
       <c r="O87" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>70.967812503065915</v>
+        <v>56.601869229698259</v>
       </c>
       <c r="P87" s="29" t="s">
         <v>249</v>
@@ -17280,7 +17280,7 @@
       </c>
       <c r="S87" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>105.21781250306591</v>
+        <v>90.851869229698252</v>
       </c>
       <c r="T87" s="5">
         <v>0</v>
@@ -17400,7 +17400,7 @@
       </c>
       <c r="O89" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>10.001217556579114</v>
+        <v>2.943450952893456</v>
       </c>
       <c r="P89" s="27" t="s">
         <v>249</v>
@@ -17414,7 +17414,7 @@
       </c>
       <c r="S89" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>60.751217556579114</v>
+        <v>53.693450952893457</v>
       </c>
       <c r="T89" s="26" t="s">
         <v>235</v>
@@ -17537,7 +17537,7 @@
       </c>
       <c r="O91" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>16.648485893013749</v>
+        <v>1.0829377694966733</v>
       </c>
       <c r="P91" s="26" t="s">
         <v>250</v>
@@ -17551,7 +17551,7 @@
       </c>
       <c r="S91" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>48.898485893013749</v>
+        <v>33.332937769496674</v>
       </c>
       <c r="T91" s="5" t="s">
         <v>37</v>
@@ -17842,7 +17842,7 @@
       </c>
       <c r="O96" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>82.924642966298478</v>
+        <v>90.062181801797465</v>
       </c>
       <c r="P96" s="29" t="s">
         <v>248</v>
@@ -17856,7 +17856,7 @@
       </c>
       <c r="S96" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>82.924642966298478</v>
+        <v>90.062181801797465</v>
       </c>
       <c r="V96" s="5" t="s">
         <v>145</v>
@@ -17913,7 +17913,7 @@
       </c>
       <c r="O97" s="35">
         <f ca="1">RAND()*(119-80)+80</f>
-        <v>89.513861799055036</v>
+        <v>82.532413951779034</v>
       </c>
       <c r="P97" s="29" t="s">
         <v>248</v>
@@ -17927,7 +17927,7 @@
       </c>
       <c r="S97" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>130.51386179905504</v>
+        <v>123.53241395177903</v>
       </c>
       <c r="V97" s="5" t="s">
         <v>145</v>
@@ -18046,7 +18046,7 @@
       </c>
       <c r="O99" s="35">
         <f ca="1">RAND()*(79-50)+50</f>
-        <v>61.130196959359424</v>
+        <v>62.770734236607865</v>
       </c>
       <c r="P99" s="29" t="s">
         <v>248</v>
@@ -18060,7 +18060,7 @@
       </c>
       <c r="S99" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>125.38019695935942</v>
+        <v>127.02073423660786</v>
       </c>
       <c r="T99" s="5" t="s">
         <v>133</v>
@@ -18176,7 +18176,7 @@
       </c>
       <c r="O101" s="35">
         <f ca="1">RAND()*(49-20)+20</f>
-        <v>43.694337130762392</v>
+        <v>43.239989156836678</v>
       </c>
       <c r="P101" s="29" t="s">
         <v>250</v>
@@ -18190,7 +18190,7 @@
       </c>
       <c r="S101" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>51.694337130762392</v>
+        <v>51.239989156836678</v>
       </c>
       <c r="T101" s="26" t="s">
         <v>239</v>
@@ -18315,7 +18315,7 @@
       </c>
       <c r="O103" s="35">
         <f ca="1">RAND()*(19-0)+0</f>
-        <v>8.3357952728733071</v>
+        <v>0.90961379949759247</v>
       </c>
       <c r="P103" s="26" t="s">
         <v>250</v>
@@ -18329,7 +18329,7 @@
       </c>
       <c r="S103" s="36">
         <f t="shared" ca="1" si="16"/>
-        <v>48.585795272873305</v>
+        <v>41.159613799497592</v>
       </c>
       <c r="T103" s="5" t="s">
         <v>137</v>
@@ -21699,10 +21699,10 @@
   <dimension ref="A1:V119"/>
   <sheetViews>
     <sheetView zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="11" ySplit="16" topLeftCell="U101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="16" topLeftCell="U17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:D103"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28265,8 +28265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA127177-25C6-664D-9F19-42DDA7C8C436}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>